<commit_message>
updated excel and pdf
Signed-off-by: Andreas Grabner <grabnerandi@gmx.at>
</commit_message>
<xml_diff>
--- a/cloudautomation/WorkshopHandsOnFEEDBACK.xlsx
+++ b/cloudautomation/WorkshopHandsOnFEEDBACK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\keptn-sandbox\keptn-on-k3s\cloudautomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dynatrace-my.sharepoint.com/personal/andreas_grabner_dynatrace_com/Documents/WORKSHOPS/CloudAutomationWorkshopsNov2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5038E4-D4CF-4093-93AB-99315389B6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="8_{5A268AEB-6642-4545-A4FF-BAE8D49D105A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42E05585-F04E-4A4D-B57B-758866C60474}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1A191AC-7BD5-41B5-8601-AF3786405756}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
-  <si>
-    <t>Andreas Grabner</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Attendee</t>
   </si>
@@ -84,54 +81,12 @@
     <t>Andi does stuff</t>
   </si>
   <si>
-    <t>Understand how to set Git Upstream for a Cloud Automationproject</t>
-  </si>
-  <si>
-    <t>Customize SLI.yaml &amp; SLO.yaml via Git Interface</t>
-  </si>
-  <si>
-    <t>Execute Quality Gate with modified SLI / SLO.yaml</t>
-  </si>
-  <si>
-    <t>Codify Quality Gates</t>
-  </si>
-  <si>
-    <t>Triggered Build 2.0.0 with failing Quality Gate</t>
-  </si>
-  <si>
-    <t>Triggered Build 3.0.0 successfully all the way to production</t>
-  </si>
-  <si>
-    <t>Triggered Build 4.0.0 directly into production</t>
-  </si>
-  <si>
-    <t>Cloud Native</t>
-  </si>
-  <si>
     <t>Created the SLO based on Synthetic Availablity</t>
   </si>
   <si>
     <t>Created SLO based on Response Time</t>
   </si>
   <si>
-    <t>Created an SLO dashboard</t>
-  </si>
-  <si>
-    <t>DevOps</t>
-  </si>
-  <si>
-    <t>Understnad how to integrate Cloud Automation with your CI/CD Tools</t>
-  </si>
-  <si>
-    <t>Monaco &amp; Release Inventory</t>
-  </si>
-  <si>
-    <t>Understand the basics behind Monaco and where to look for more</t>
-  </si>
-  <si>
-    <t>Understand the basics behind Release Inventory and where to look for more</t>
-  </si>
-  <si>
     <t>aapl</t>
   </si>
   <si>
@@ -249,9 +204,6 @@
     <t>Release Validation</t>
   </si>
   <si>
-    <t>Create/Clone your Release Validation Dashboard</t>
-  </si>
-  <si>
     <t>Trigger an evaluation for Release A</t>
   </si>
   <si>
@@ -262,12 +214,6 @@
   </si>
   <si>
     <t>Delivery Pipelines</t>
-  </si>
-  <si>
-    <t>Create / Clone your SLO-based Quality Gate Dashboard for staging</t>
-  </si>
-  <si>
-    <t>Trigger new deployments and validate dashboard is used</t>
   </si>
   <si>
     <t>Validate results and events in Dynatrace release monitoring</t>
@@ -343,28 +289,40 @@
     </r>
   </si>
   <si>
-    <t>Access Keptn CLI. Either locally, through SSH or through the Bastion Web</t>
-  </si>
-  <si>
     <t>Break</t>
   </si>
   <si>
     <t>Back from your break?</t>
   </si>
   <si>
-    <t>username for attendees</t>
-  </si>
-  <si>
-    <t>passwordforattendees</t>
-  </si>
-  <si>
-    <t>password for attendees</t>
-  </si>
-  <si>
-    <t>https://yourcloudautomationtenantlink</t>
-  </si>
-  <si>
-    <t>https://yourdynatracetenantlink</t>
+    <t>Simple CI/CD Automation Trigger</t>
+  </si>
+  <si>
+    <t>Access Cloud Automation UI and "Sample DevOps Tools"</t>
+  </si>
+  <si>
+    <t>https://abc12345.live.dynatrace.com</t>
+  </si>
+  <si>
+    <t>https://abc12345.cloudautomation.live.dynatrace.com/</t>
+  </si>
+  <si>
+    <t>http://keptnwebservice.keptnwebservice-production.YOURDOMAIN/</t>
+  </si>
+  <si>
+    <t>Created an SLO dashboard - or let Monaco create SLO for you</t>
+  </si>
+  <si>
+    <t>Create Release Validation Dashboard or let Monaco create it for you</t>
+  </si>
+  <si>
+    <t>Update SLO.yaml for your service</t>
+  </si>
+  <si>
+    <t>Trigger new deployments and validate SLO.yaml is used</t>
+  </si>
+  <si>
+    <t>INSTRUCTOR NAME</t>
   </si>
 </sst>
 </file>
@@ -492,7 +450,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -514,19 +472,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -593,7 +538,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -624,16 +569,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -646,13 +584,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -664,20 +596,18 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -996,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4DFDDD-899D-4204-A93E-75BF87DA9C59}">
-  <dimension ref="A1:AJ47"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,217 +937,155 @@
     <col min="1" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="9" width="18.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="7" customWidth="1"/>
-    <col min="11" max="13" width="20.42578125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="12" style="7" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="7" customWidth="1"/>
-    <col min="17" max="19" width="18.85546875" style="7" customWidth="1"/>
+    <col min="5" max="8" width="18.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="7" customWidth="1"/>
+    <col min="10" max="12" width="20.42578125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="12" style="7" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" style="7" customWidth="1"/>
+    <col min="16" max="19" width="18.85546875" style="7" customWidth="1"/>
     <col min="20" max="20" width="4.7109375" style="7" customWidth="1"/>
-    <col min="21" max="23" width="18.85546875" style="7" customWidth="1"/>
-    <col min="24" max="24" width="5" style="7" customWidth="1"/>
-    <col min="25" max="27" width="18.85546875" style="7" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" style="7" customWidth="1"/>
-    <col min="29" max="29" width="18.85546875" style="7" customWidth="1"/>
-    <col min="30" max="30" width="3.85546875" style="7" customWidth="1"/>
-    <col min="31" max="33" width="18.85546875" customWidth="1"/>
-    <col min="34" max="34" width="3.5703125" customWidth="1"/>
-    <col min="35" max="36" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" customWidth="1"/>
+    <col min="23" max="23" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="27"/>
+    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="H2" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>88</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="16"/>
       <c r="S4"/>
       <c r="T4"/>
-      <c r="U4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
       <c r="S5"/>
       <c r="T5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E6"/>
-      <c r="G6"/>
-      <c r="H6" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="G6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
       <c r="S6"/>
       <c r="T6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="G7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
       <c r="S7"/>
       <c r="T7"/>
-      <c r="U7"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D8" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>87</v>
-      </c>
+      <c r="G8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
       <c r="O8"/>
-      <c r="P8"/>
       <c r="S8"/>
       <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
@@ -1229,51 +1097,33 @@
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9"/>
-      <c r="P9"/>
       <c r="S9"/>
       <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E10"/>
       <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="26"/>
+      <c r="G10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
       <c r="O10"/>
-      <c r="P10"/>
       <c r="S10"/>
       <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11" s="21"/>
+      <c r="H11" s="18"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1281,32 +1131,19 @@
       <c r="M11"/>
       <c r="N11"/>
       <c r="O11"/>
-      <c r="P11"/>
       <c r="S11"/>
       <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>79</v>
-      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="26" t="s">
-        <v>81</v>
-      </c>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12" s="21"/>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>63</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1319,19 +1156,9 @@
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C13" s="26"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C13" s="21"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -1348,454 +1175,352 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-    </row>
-    <row r="14" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="32"/>
-      <c r="J14"/>
-      <c r="K14" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="33"/>
-      <c r="M14" s="32"/>
-      <c r="N14"/>
-      <c r="O14" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="P14"/>
-      <c r="Q14" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="R14" s="33"/>
-      <c r="S14" s="32"/>
+    </row>
+    <row r="14" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14"/>
+      <c r="J14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="27"/>
+      <c r="M14"/>
+      <c r="N14" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="O14"/>
+      <c r="P14" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="27"/>
       <c r="T14"/>
-      <c r="U14" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="V14" s="33"/>
-      <c r="W14" s="32"/>
-      <c r="X14"/>
-      <c r="Y14" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="32"/>
-      <c r="AC14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD14"/>
-      <c r="AE14" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF14" s="33"/>
-      <c r="AG14" s="32"/>
-      <c r="AI14" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ14" s="32"/>
-    </row>
-    <row r="15" spans="1:36" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U14" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="V14" s="28"/>
+      <c r="W14" s="27"/>
+    </row>
+    <row r="15" spans="1:23" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15"/>
+      <c r="N15" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="11" t="s">
+      <c r="O15"/>
+      <c r="P15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15"/>
-      <c r="K15" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15"/>
-      <c r="O15" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="P15"/>
-      <c r="Q15" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="R15" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="S15" s="22" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="T15"/>
       <c r="U15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="V15" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="W15" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>76</v>
       </c>
-      <c r="V15" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="W15" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z15" s="12" t="s">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="AA15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD15"/>
-      <c r="AE15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG15" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ15" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="25"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D45"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="18"/>
-      <c r="AA45" s="18"/>
-      <c r="AB45" s="18"/>
-      <c r="AC45" s="18"/>
-      <c r="AD45" s="18"/>
-    </row>
-    <row r="46" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+    </row>
+    <row r="46" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="18"/>
-      <c r="Z46" s="18"/>
-      <c r="AA46" s="18"/>
-      <c r="AB46" s="18"/>
-      <c r="AC46" s="18"/>
-      <c r="AD46" s="18"/>
-    </row>
-    <row r="47" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+    </row>
+    <row r="47" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
-      <c r="W47" s="18"/>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="18"/>
-      <c r="AA47" s="18"/>
-      <c r="AB47" s="18"/>
-      <c r="AC47" s="18"/>
-      <c r="AD47" s="18"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="K14:M14"/>
+  <mergeCells count="4">
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="U14:W14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" xr:uid="{D5F33484-CED7-4A1C-B15E-73C20D29BB99}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{FB40B47A-E508-4911-8E1F-D0F68F3B1C65}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{F3403990-B684-4D31-8BB2-28234168AA33}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{FFFD2042-1BF6-45EC-BCDB-C9DC4237FBBC}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{D5F33484-CED7-4A1C-B15E-73C20D29BB99}"/>
+    <hyperlink ref="H12" r:id="rId3" xr:uid="{FB40B47A-E508-4911-8E1F-D0F68F3B1C65}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{C63C8201-8ADA-43DF-A0C8-98C63DBB541C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>